<commit_message>
java class and methods are updated.
</commit_message>
<xml_diff>
--- a/20506_Java_Class&Methods/Class&Methods.xlsx
+++ b/20506_Java_Class&Methods/Class&Methods.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sonata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sonata\sonata_case_study\20506_Java_Class&amp;Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE038940-15BB-433E-B396-BAF7EC8AAD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E471BC03-8C60-41AB-AFBD-B30645647EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6708EFF7-7B71-4F7E-B6DE-B23D115DAD01}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -162,18 +162,9 @@
     <t>bookSlot(pat,dr,date,from,to)</t>
   </si>
   <si>
-    <t>deleteSlot(slot_id)</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>docLogin(docId, password)</t>
-  </si>
-  <si>
-    <t>patLogin(patId, password)</t>
-  </si>
-  <si>
     <t>forgotPassword(docId/patId)</t>
   </si>
   <si>
@@ -187,6 +178,9 @@
   </si>
   <si>
     <t>panndingSlots()</t>
+  </si>
+  <si>
+    <t>Login(docId/patid, password)</t>
   </si>
 </sst>
 </file>
@@ -210,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,8 +259,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -274,15 +274,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -291,6 +368,22 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EBF051-B0EA-420D-8904-784705BD135F}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,307 +719,312 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K7" s="4"/>
-      <c r="L7" s="4" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C19" s="8"/>
+      <c r="C19" s="7"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="9" t="s">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="11"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C35" s="5" t="s">
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="18"/>
+      <c r="C35" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C36" s="7" t="s">
+      <c r="E35" s="17"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="19"/>
+      <c r="C36" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="9" t="s">
+      <c r="D36" s="21"/>
+      <c r="E36" s="22"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C40" s="7" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C40" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="9" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C44" s="5" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C44" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C45" s="5" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C45" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C46" s="5" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C46" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C47" s="7" t="s">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C47" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C48" s="7" t="s">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C48" s="10"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="9" t="s">
+      <c r="C51" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C52" s="5" t="s">
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C53" s="5" t="s">
+      <c r="C57" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C58" s="6" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C54" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C58" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>